<commit_message>
writing the count and match string along with ignoring the string case and string sequence
</commit_message>
<xml_diff>
--- a/best_matching_images.xlsx
+++ b/best_matching_images.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,6 +441,11 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Match Count</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Image</t>
         </is>
       </c>
@@ -451,7 +456,10 @@
           <t>string_list1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>page_20.png</t>
         </is>
@@ -463,7 +471,10 @@
           <t>string_list1</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>page_21.png</t>
         </is>
@@ -475,7 +486,10 @@
           <t>string_list1</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>page_22.png</t>
         </is>
@@ -487,7 +501,10 @@
           <t>string_list1</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>page_23.png</t>
         </is>
@@ -499,7 +516,10 @@
           <t>string_list1</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t>page_24.png</t>
         </is>
@@ -508,12 +528,15 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>string_list1</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>page_25.png</t>
+          <t>string_list2</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>page_24.png</t>
         </is>
       </c>
     </row>
@@ -523,21 +546,27 @@
           <t>string_list1</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>page_26.png</t>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>page_25.png</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>string_list1</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>page_27.png</t>
+          <t>string_list2</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>page_25.png</t>
         </is>
       </c>
     </row>
@@ -547,21 +576,27 @@
           <t>string_list1</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>page_30.png</t>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>page_26.png</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>string_list1</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>page_31.png</t>
+          <t>string_list2</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>page_26.png</t>
         </is>
       </c>
     </row>
@@ -571,69 +606,87 @@
           <t>string_list1</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>page_32.png</t>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>page_27.png</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>string_list1</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>page_4.png</t>
+          <t>string_list2</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>page_29.png</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>string_list2</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>page_24.png</t>
+          <t>string_list1</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>page_30.png</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>string_list2</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>page_25.png</t>
+          <t>string_list1</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>page_31.png</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>string_list2</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>page_26.png</t>
+          <t>string_list1</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>page_32.png</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>string_list2</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>page_29.png</t>
+          <t>string_list1</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>page_4.png</t>
         </is>
       </c>
     </row>
@@ -643,7 +696,10 @@
           <t>string_list2</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
         <is>
           <t>page_6.png</t>
         </is>
@@ -655,321 +711,12 @@
           <t>string_list2</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" t="inlineStr">
         <is>
           <t>text.jpg</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>page_10.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>page_11.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>page_12.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>page_13.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>page_14.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>page_15.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>page_17.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>page_18.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>page_19.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>page_20.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>page_21.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>page_22.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>page_23.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>page_24.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>page_25.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>page_26.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>page_27.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>page_28.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>page_30.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>page_32.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>page_4.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>page_5.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>page_6.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>page_7.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>page_8.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>string_list3</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>page_9.png</t>
         </is>
       </c>
     </row>

</xml_diff>